<commit_message>
further refining board size, adding rotary encoder and OLED display
</commit_message>
<xml_diff>
--- a/minipowersupply.xlsx
+++ b/minipowersupply.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\electronics\mini-power-supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46ED3714-DF14-4874-95A1-1C1E08D08830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01C59A-12D7-49E3-9610-04355AA56768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240"/>
+    <workbookView xWindow="24765" yWindow="375" windowWidth="17025" windowHeight="17430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="minipowersupply" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="136">
   <si>
     <t>Source:</t>
   </si>
@@ -377,13 +391,64 @@
   </si>
   <si>
     <t>Dual operational amplifier</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>U-</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>U+</t>
+  </si>
+  <si>
+    <t>A0..2</t>
+  </si>
+  <si>
+    <t>A3..5</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>D7..12</t>
+  </si>
+  <si>
+    <t>5+</t>
+  </si>
+  <si>
+    <t>Meas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,8 +583,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,8 +780,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -815,6 +902,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -860,9 +1058,45 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -908,7 +1142,139 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -919,6 +1285,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0393E7BD-9100-4B32-8FB0-5C15C617B769}" name="Table1" displayName="Table1" ref="A9:D14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A9:D14" xr:uid="{0393E7BD-9100-4B32-8FB0-5C15C617B769}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6513DE97-F392-49E9-B34A-8857CC3D9080}" name="Meas" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{58C57F97-74C0-439B-8EE8-3221BBFC98B2}" name="A0..2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7940FB4F-4FB9-4EA8-B447-A2CF6BF3F445}" name="A3..5" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{BCF4F6D9-2256-460F-8DAD-E4C7FEF5DB1F}" name="D7..12" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT(B10:C10)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1217,10 +1598,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1917,4 +2298,203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287DDBB7-1C31-4941-A248-D99353000EFE}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="A8:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f>_xlfn.CONCAT(B10:C10)</f>
+        <v>011100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" ref="D11:D14" si="0">_xlfn.CONCAT(B11:C11)</f>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>001010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>010011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>100001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding diff and summing amps to scale amp inputs
</commit_message>
<xml_diff>
--- a/minipowersupply.xlsx
+++ b/minipowersupply.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\electronics\mini-power-supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01C59A-12D7-49E3-9610-04355AA56768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52B4727-69EA-410A-8D19-2E888434BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24765" yWindow="375" windowWidth="17025" windowHeight="17430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24915" yWindow="1470" windowWidth="20760" windowHeight="17430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="minipowersupply" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="135">
   <si>
     <t>Source:</t>
   </si>
@@ -421,9 +421,6 @@
   </si>
   <si>
     <t>011</t>
-  </si>
-  <si>
-    <t>100</t>
   </si>
   <si>
     <t>000</t>
@@ -1144,35 +1141,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1253,13 +1221,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1272,6 +1233,42 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1288,13 +1285,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0393E7BD-9100-4B32-8FB0-5C15C617B769}" name="Table1" displayName="Table1" ref="A9:D14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0393E7BD-9100-4B32-8FB0-5C15C617B769}" name="Table1" displayName="Table1" ref="A9:D14" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A9:D14" xr:uid="{0393E7BD-9100-4B32-8FB0-5C15C617B769}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6513DE97-F392-49E9-B34A-8857CC3D9080}" name="Meas" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{58C57F97-74C0-439B-8EE8-3221BBFC98B2}" name="A0..2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7940FB4F-4FB9-4EA8-B447-A2CF6BF3F445}" name="A3..5" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{BCF4F6D9-2256-460F-8DAD-E4C7FEF5DB1F}" name="D7..12" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{6513DE97-F392-49E9-B34A-8857CC3D9080}" name="Meas" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{58C57F97-74C0-439B-8EE8-3221BBFC98B2}" name="A0..2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{7940FB4F-4FB9-4EA8-B447-A2CF6BF3F445}" name="A3..5" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BCF4F6D9-2256-460F-8DAD-E4C7FEF5DB1F}" name="D7..12" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(B10:C10)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2305,7 +2302,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="A8:D14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,10 +2327,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -2345,7 +2342,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -2354,10 +2351,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2365,11 +2362,11 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>124</v>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2378,7 +2375,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>125</v>
@@ -2403,7 +2400,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>126</v>
@@ -2412,22 +2409,22 @@
         <v>127</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>129</v>
+      <c r="B10" s="5">
+        <v>100</v>
+      </c>
+      <c r="C10" s="5">
+        <v>100</v>
       </c>
       <c r="D10" s="7" t="str">
         <f>_xlfn.CONCAT(B10:C10)</f>
-        <v>011100</v>
+        <v>100100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,14 +2432,14 @@
         <v>122</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D11" s="7" t="str">
         <f t="shared" ref="D11:D14" si="0">_xlfn.CONCAT(B11:C11)</f>
-        <v>000000</v>
+        <v>010010</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,14 +2447,14 @@
         <v>123</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>001010</v>
+        <v>001000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,29 +2462,29 @@
         <v>124</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>010011</v>
+        <v>000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>100001</v>
+        <v>011011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>